<commit_message>
Excel samle column demo
</commit_message>
<xml_diff>
--- a/Sample Columns.xlsx
+++ b/Sample Columns.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF2780D-0593-4D2C-BC45-114FBF435013}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,101 +370,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>159</v>
       </c>
       <c r="B1">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3359</v>
       </c>
       <c r="B2">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>3394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9072</v>
       </c>
       <c r="B3">
         <v>8996</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>18068</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>623</v>
       </c>
       <c r="B4">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
       <c r="B5">
         <v>324</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6643</v>
       </c>
       <c r="B6">
         <v>88942</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>95585</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3213</v>
       </c>
       <c r="B8">
         <v>4324</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>7537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7732</v>
       </c>
       <c r="B9">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>7775</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>952</v>
       </c>
       <c r="B10">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3577</v>
       </c>
       <c r="B11">
         <v>91</v>
+      </c>
+      <c r="C11">
+        <v>3668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>